<commit_message>
changed some input data
</commit_message>
<xml_diff>
--- a/data/input_operation/OperationScenario_Component_HeatingElement.xlsx
+++ b/data/input_operation/OperationScenario_Component_HeatingElement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mascherbauer\PycharmProjects\NewTrends\Prosumager\data\input_operation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860F17A5-330F-480E-944C-18009A347D1A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D95211-441C-4CBC-BBA5-DB3439310FF1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="19200" windowHeight="6360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="765" windowWidth="19200" windowHeight="6360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OperationScenario_Component_Hea" sheetId="1" r:id="rId1"/>
@@ -881,12 +881,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -900,12 +900,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>

</xml_diff>